<commit_message>
added drag polars for takeoff and landing
under flap_sizing_main_playaround
</commit_message>
<xml_diff>
--- a/drag_buildup_flap_sizing/initial_flap_comparison.xlsx
+++ b/drag_buildup_flap_sizing/initial_flap_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tysonc/Documents/GitHub/443_design_problem/drag_buildup_flap_sizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC393A36-8FFB-EA44-AB98-979E3F29AE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422EB5CC-4CBF-B34F-A7BF-D7F73FD55313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{EC71E661-8E68-AE42-9A06-41E38954078A}"/>
+    <workbookView xWindow="21580" yWindow="760" windowWidth="12980" windowHeight="21100" xr2:uid="{EC71E661-8E68-AE42-9A06-41E38954078A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,10 +60,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8231964C-65AC-874E-94E0-85B4CCD0BDA9}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,6 +456,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
       <c r="B2">
         <v>-0.160833112563248</v>
       </c>
@@ -459,6 +470,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>35</v>
+      </c>
       <c r="B3">
         <v>-0.24489211663778099</v>
       </c>
@@ -470,6 +484,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>40</v>
+      </c>
       <c r="B4">
         <v>-0.311134863511149</v>
       </c>
@@ -481,6 +498,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>45</v>
+      </c>
       <c r="B5">
         <v>-0.36209132500913099</v>
       </c>
@@ -492,6 +512,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>50</v>
+      </c>
       <c r="B6">
         <v>-0.39092967389987998</v>
       </c>
@@ -502,9 +525,14 @@
         <v>0.136296463380191</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
+      <c r="A10" s="1">
+        <v>30</v>
       </c>
       <c r="B10">
         <v>-0.12273920085638799</v>
@@ -517,6 +545,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>35</v>
+      </c>
       <c r="B11">
         <v>-0.197461182222815</v>
       </c>
@@ -528,6 +559,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>40</v>
+      </c>
       <c r="B12">
         <v>-0.23906765116337</v>
       </c>
@@ -539,6 +573,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45</v>
+      </c>
       <c r="B13">
         <v>-0.27668634208838799</v>
       </c>
@@ -550,6 +587,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>50</v>
+      </c>
       <c r="B14">
         <v>-0.32270154761312803</v>
       </c>
@@ -566,6 +606,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>30</v>
+      </c>
       <c r="B18">
         <v>-6.6322043718229598E-2</v>
       </c>
@@ -577,6 +620,9 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>35</v>
+      </c>
       <c r="B19">
         <v>-0.130149249651235</v>
       </c>
@@ -588,6 +634,9 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>40</v>
+      </c>
       <c r="B20">
         <v>-0.19037211794960901</v>
       </c>
@@ -599,6 +648,9 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>45</v>
+      </c>
       <c r="B21">
         <v>-0.25046813640266802</v>
       </c>
@@ -610,6 +662,9 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>50</v>
+      </c>
       <c r="B22">
         <v>-0.30724264125893103</v>
       </c>

</xml_diff>